<commit_message>
Completed refactor to read excel using Excel-IO library
</commit_message>
<xml_diff>
--- a/SpreadsheetConsole/TestSheet.xlsx
+++ b/SpreadsheetConsole/TestSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20350"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stmartin.edu\dfs\users\zachary.michaels\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\izmac\source\repos\emailConfirmationAssistant-1\SpreadsheetConsole\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F41D798-2114-48FE-B09D-3FE9A76A6A8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D17C3C-0D77-4E30-8A17-5F8FE2A2C9DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11010" xr2:uid="{227B31AE-315F-4CFF-8A71-775C54A0AB13}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{227B31AE-315F-4CFF-8A71-775C54A0AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>kimberly.castro13@outlook.com</t>
   </si>
@@ -117,16 +117,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -145,8 +153,8 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9F0AA9F0-9947-4842-BC7C-0C789CABC693}" name="FirstName"/>
     <tableColumn id="4" xr3:uid="{F7C1D84E-18ED-458E-8F05-A036C7F4A1A8}" name="LastName"/>
-    <tableColumn id="2" xr3:uid="{FC69B1F1-3BAD-4130-A755-B608D1D33DE7}" name="Outlook" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{4FD99D7B-4F3B-40CD-9DF7-322BAF0AA297}" name="StMartin" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{FC69B1F1-3BAD-4130-A755-B608D1D33DE7}" name="Outlook" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{4FD99D7B-4F3B-40CD-9DF7-322BAF0AA297}" name="StMartin" dataDxfId="0" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -452,7 +460,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,10 +492,10 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -501,7 +509,7 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -523,14 +531,12 @@
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{A0E63DEF-40D1-4EF5-B46E-21934C3F13F1}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{1180B84A-C734-4A35-9A2B-5768EF1176E5}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{2E54B438-85FA-4884-B196-02EA711D608E}"/>
-    <hyperlink ref="D2" r:id="rId4" xr:uid="{826CA2D7-7897-4F11-BA50-C65F07DB2548}"/>
-    <hyperlink ref="C4" r:id="rId5" xr:uid="{5C7464A9-C7DF-4AA8-8E3F-F794106123E1}"/>
-    <hyperlink ref="D4" r:id="rId6" xr:uid="{55AAEE8A-99FA-4361-90FE-8174BCDAE5D6}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{5C7464A9-C7DF-4AA8-8E3F-F794106123E1}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{55AAEE8A-99FA-4361-90FE-8174BCDAE5D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>